<commit_message>
Updated Project with Daily usage pattern
</commit_message>
<xml_diff>
--- a/Project/Data Set 1 - All Day Usage - 30 Min Interval Data.xlsx
+++ b/Project/Data Set 1 - All Day Usage - 30 Min Interval Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\1. ATU Galway - BSc in Computing (Data Analytics)\3. Sem-2 Programming for Data Analytics\2. PFDA Weekly Tasks &amp; Labs - Project\12. Project\1. Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAD-PC\Desktop\GitHub - Cloned Repository\PFDA\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8B0C3D-6FDA-4FBE-B743-98552AD59AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDED454-72E8-41D6-81CF-B25B371053F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,25 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>TOTAL 30 Min Interval Data</t>
-  </si>
-  <si>
-    <t>Total Annual Consumption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0&quot;kWh&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0&quot;kWh&quot;"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,7 +74,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,59 +97,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW369"/>
+  <dimension ref="A1:AW365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="A368" sqref="A368"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A362" sqref="A362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,157 +398,157 @@
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5">
+    <row r="1" spans="1:49" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="3">
         <v>0.125</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="3">
         <v>0.1875</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="3">
         <v>0.22916666666666666</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="3">
         <v>0.25</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="3">
         <v>0.27083333333333331</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="3">
         <v>0.29166666666666669</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="3">
         <v>0.3125</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="3">
         <v>0.35416666666666669</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="3">
         <v>0.375</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="3">
         <v>0.4375</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="3">
         <v>0.47916666666666669</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="3">
         <v>0.5</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="3">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AC1" s="3">
         <v>0.5625</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AD1" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AE1" s="3">
         <v>0.60416666666666663</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AF1" s="3">
         <v>0.625</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AG1" s="3">
         <v>0.64583333333333337</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AH1" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AI1" s="3">
         <v>0.6875</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AJ1" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AK1" s="3">
         <v>0.72916666666666663</v>
       </c>
-      <c r="AL1" s="5">
+      <c r="AL1" s="3">
         <v>0.75</v>
       </c>
-      <c r="AM1" s="5">
+      <c r="AM1" s="3">
         <v>0.77083333333333337</v>
       </c>
-      <c r="AN1" s="5">
+      <c r="AN1" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="AO1" s="5">
+      <c r="AO1" s="3">
         <v>0.8125</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AP1" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="AQ1" s="5">
+      <c r="AQ1" s="3">
         <v>0.85416666666666663</v>
       </c>
-      <c r="AR1" s="5">
+      <c r="AR1" s="3">
         <v>0.875</v>
       </c>
-      <c r="AS1" s="5">
+      <c r="AS1" s="3">
         <v>0.89583333333333337</v>
       </c>
-      <c r="AT1" s="5">
+      <c r="AT1" s="3">
         <v>0.91666666666666663</v>
       </c>
-      <c r="AU1" s="5">
+      <c r="AU1" s="3">
         <v>0.9375</v>
       </c>
-      <c r="AV1" s="5">
+      <c r="AV1" s="3">
         <v>0.95833333333333337</v>
       </c>
-      <c r="AW1" s="5">
+      <c r="AW1" s="3">
         <v>0.97916666666666663</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>45624</v>
       </c>
       <c r="B2">
@@ -750,7 +697,7 @@
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45625</v>
       </c>
       <c r="B3">
@@ -899,7 +846,7 @@
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>45626</v>
       </c>
       <c r="B4">
@@ -1048,7 +995,7 @@
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>45627</v>
       </c>
       <c r="B5">
@@ -1197,7 +1144,7 @@
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>45628</v>
       </c>
       <c r="B6">
@@ -1346,7 +1293,7 @@
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>45629</v>
       </c>
       <c r="B7">
@@ -1495,7 +1442,7 @@
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>45630</v>
       </c>
       <c r="B8">
@@ -1644,7 +1591,7 @@
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>45631</v>
       </c>
       <c r="B9">
@@ -1793,7 +1740,7 @@
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>45632</v>
       </c>
       <c r="B10">
@@ -1942,7 +1889,7 @@
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>45633</v>
       </c>
       <c r="B11">
@@ -2091,7 +2038,7 @@
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>45634</v>
       </c>
       <c r="B12">
@@ -2240,7 +2187,7 @@
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>45635</v>
       </c>
       <c r="B13">
@@ -2389,7 +2336,7 @@
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>45636</v>
       </c>
       <c r="B14">
@@ -2538,7 +2485,7 @@
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>45637</v>
       </c>
       <c r="B15">
@@ -2687,7 +2634,7 @@
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>45638</v>
       </c>
       <c r="B16">
@@ -2836,7 +2783,7 @@
       </c>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>45639</v>
       </c>
       <c r="B17">
@@ -2985,7 +2932,7 @@
       </c>
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>45640</v>
       </c>
       <c r="B18">
@@ -3134,7 +3081,7 @@
       </c>
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>45641</v>
       </c>
       <c r="B19">
@@ -3283,7 +3230,7 @@
       </c>
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>45642</v>
       </c>
       <c r="B20">
@@ -3432,7 +3379,7 @@
       </c>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>45643</v>
       </c>
       <c r="B21">
@@ -3581,7 +3528,7 @@
       </c>
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>45644</v>
       </c>
       <c r="B22">
@@ -3730,7 +3677,7 @@
       </c>
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>45645</v>
       </c>
       <c r="B23">
@@ -3879,7 +3826,7 @@
       </c>
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>45646</v>
       </c>
       <c r="B24">
@@ -4028,7 +3975,7 @@
       </c>
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>45647</v>
       </c>
       <c r="B25">
@@ -4177,7 +4124,7 @@
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>45648</v>
       </c>
       <c r="B26">
@@ -4326,7 +4273,7 @@
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>45649</v>
       </c>
       <c r="B27">
@@ -4475,7 +4422,7 @@
       </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>45650</v>
       </c>
       <c r="B28">
@@ -4624,7 +4571,7 @@
       </c>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>45651</v>
       </c>
       <c r="B29">
@@ -4773,7 +4720,7 @@
       </c>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>45652</v>
       </c>
       <c r="B30">
@@ -4922,7 +4869,7 @@
       </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>45653</v>
       </c>
       <c r="B31">
@@ -5071,7 +5018,7 @@
       </c>
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>45654</v>
       </c>
       <c r="B32">
@@ -5220,7 +5167,7 @@
       </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>45655</v>
       </c>
       <c r="B33">
@@ -5369,7 +5316,7 @@
       </c>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>45656</v>
       </c>
       <c r="B34">
@@ -5518,7 +5465,7 @@
       </c>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>45657</v>
       </c>
       <c r="B35">
@@ -5667,7 +5614,7 @@
       </c>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>45658</v>
       </c>
       <c r="B36">
@@ -5816,7 +5763,7 @@
       </c>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>45659</v>
       </c>
       <c r="B37">
@@ -5965,7 +5912,7 @@
       </c>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>45660</v>
       </c>
       <c r="B38">
@@ -6114,7 +6061,7 @@
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>45661</v>
       </c>
       <c r="B39">
@@ -6263,7 +6210,7 @@
       </c>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>45662</v>
       </c>
       <c r="B40">
@@ -6412,7 +6359,7 @@
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>45663</v>
       </c>
       <c r="B41">
@@ -6561,7 +6508,7 @@
       </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>45664</v>
       </c>
       <c r="B42">
@@ -6710,7 +6657,7 @@
       </c>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>45665</v>
       </c>
       <c r="B43">
@@ -6859,7 +6806,7 @@
       </c>
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>45666</v>
       </c>
       <c r="B44">
@@ -7008,7 +6955,7 @@
       </c>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>45667</v>
       </c>
       <c r="B45">
@@ -7157,7 +7104,7 @@
       </c>
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>45668</v>
       </c>
       <c r="B46">
@@ -7306,7 +7253,7 @@
       </c>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>45669</v>
       </c>
       <c r="B47">
@@ -7455,7 +7402,7 @@
       </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>45670</v>
       </c>
       <c r="B48">
@@ -7604,7 +7551,7 @@
       </c>
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>45671</v>
       </c>
       <c r="B49">
@@ -7753,7 +7700,7 @@
       </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>45672</v>
       </c>
       <c r="B50">
@@ -7902,7 +7849,7 @@
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>45673</v>
       </c>
       <c r="B51">
@@ -8051,7 +7998,7 @@
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>45674</v>
       </c>
       <c r="B52">
@@ -8200,7 +8147,7 @@
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>45675</v>
       </c>
       <c r="B53">
@@ -8349,7 +8296,7 @@
       </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>45676</v>
       </c>
       <c r="B54">
@@ -8498,7 +8445,7 @@
       </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>45677</v>
       </c>
       <c r="B55">
@@ -8647,7 +8594,7 @@
       </c>
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>45678</v>
       </c>
       <c r="B56">
@@ -8796,7 +8743,7 @@
       </c>
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>45679</v>
       </c>
       <c r="B57">
@@ -8945,7 +8892,7 @@
       </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>45680</v>
       </c>
       <c r="B58">
@@ -9094,7 +9041,7 @@
       </c>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="1">
         <v>45681</v>
       </c>
       <c r="B59">
@@ -9243,7 +9190,7 @@
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>45682</v>
       </c>
       <c r="B60">
@@ -9392,7 +9339,7 @@
       </c>
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>45683</v>
       </c>
       <c r="B61">
@@ -9541,7 +9488,7 @@
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>45684</v>
       </c>
       <c r="B62">
@@ -9690,7 +9637,7 @@
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="1">
         <v>45685</v>
       </c>
       <c r="B63">
@@ -9839,7 +9786,7 @@
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="1">
         <v>45686</v>
       </c>
       <c r="B64">
@@ -9988,7 +9935,7 @@
       </c>
     </row>
     <row r="65" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="1">
         <v>45687</v>
       </c>
       <c r="B65">
@@ -10137,7 +10084,7 @@
       </c>
     </row>
     <row r="66" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="1">
         <v>45688</v>
       </c>
       <c r="B66">
@@ -10286,7 +10233,7 @@
       </c>
     </row>
     <row r="67" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="1">
         <v>45689</v>
       </c>
       <c r="B67">
@@ -10435,7 +10382,7 @@
       </c>
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="1">
         <v>45690</v>
       </c>
       <c r="B68">
@@ -10584,7 +10531,7 @@
       </c>
     </row>
     <row r="69" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="1">
         <v>45691</v>
       </c>
       <c r="B69">
@@ -10733,7 +10680,7 @@
       </c>
     </row>
     <row r="70" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="1">
         <v>45692</v>
       </c>
       <c r="B70">
@@ -10882,7 +10829,7 @@
       </c>
     </row>
     <row r="71" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="1">
         <v>45693</v>
       </c>
       <c r="B71">
@@ -11031,7 +10978,7 @@
       </c>
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>45694</v>
       </c>
       <c r="B72">
@@ -11180,7 +11127,7 @@
       </c>
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="1">
         <v>45695</v>
       </c>
       <c r="B73">
@@ -11329,7 +11276,7 @@
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="1">
         <v>45696</v>
       </c>
       <c r="B74">
@@ -11478,7 +11425,7 @@
       </c>
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="1">
         <v>45697</v>
       </c>
       <c r="B75">
@@ -11627,7 +11574,7 @@
       </c>
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="1">
         <v>45698</v>
       </c>
       <c r="B76">
@@ -11776,7 +11723,7 @@
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="1">
         <v>45699</v>
       </c>
       <c r="B77">
@@ -11925,7 +11872,7 @@
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="1">
         <v>45700</v>
       </c>
       <c r="B78">
@@ -12074,7 +12021,7 @@
       </c>
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="1">
         <v>45701</v>
       </c>
       <c r="B79">
@@ -12223,7 +12170,7 @@
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="1">
         <v>45702</v>
       </c>
       <c r="B80">
@@ -12372,7 +12319,7 @@
       </c>
     </row>
     <row r="81" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="1">
         <v>45703</v>
       </c>
       <c r="B81">
@@ -12521,7 +12468,7 @@
       </c>
     </row>
     <row r="82" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="1">
         <v>45704</v>
       </c>
       <c r="B82">
@@ -12670,7 +12617,7 @@
       </c>
     </row>
     <row r="83" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="1">
         <v>45705</v>
       </c>
       <c r="B83">
@@ -12819,7 +12766,7 @@
       </c>
     </row>
     <row r="84" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="1">
         <v>45706</v>
       </c>
       <c r="B84">
@@ -12968,7 +12915,7 @@
       </c>
     </row>
     <row r="85" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="1">
         <v>45707</v>
       </c>
       <c r="B85">
@@ -13117,7 +13064,7 @@
       </c>
     </row>
     <row r="86" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="1">
         <v>45708</v>
       </c>
       <c r="B86">
@@ -13266,7 +13213,7 @@
       </c>
     </row>
     <row r="87" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="1">
         <v>45709</v>
       </c>
       <c r="B87">
@@ -13415,7 +13362,7 @@
       </c>
     </row>
     <row r="88" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="1">
         <v>45710</v>
       </c>
       <c r="B88">
@@ -13564,7 +13511,7 @@
       </c>
     </row>
     <row r="89" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="1">
         <v>45711</v>
       </c>
       <c r="B89">
@@ -13713,7 +13660,7 @@
       </c>
     </row>
     <row r="90" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="1">
         <v>45712</v>
       </c>
       <c r="B90">
@@ -13862,7 +13809,7 @@
       </c>
     </row>
     <row r="91" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="1">
         <v>45713</v>
       </c>
       <c r="B91">
@@ -14011,7 +13958,7 @@
       </c>
     </row>
     <row r="92" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="1">
         <v>45714</v>
       </c>
       <c r="B92">
@@ -14160,7 +14107,7 @@
       </c>
     </row>
     <row r="93" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="1">
         <v>45715</v>
       </c>
       <c r="B93">
@@ -14309,7 +14256,7 @@
       </c>
     </row>
     <row r="94" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="1">
         <v>45716</v>
       </c>
       <c r="B94">
@@ -14458,7 +14405,7 @@
       </c>
     </row>
     <row r="95" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="1">
         <v>45717</v>
       </c>
       <c r="B95">
@@ -14607,7 +14554,7 @@
       </c>
     </row>
     <row r="96" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="1">
         <v>45718</v>
       </c>
       <c r="B96">
@@ -14756,7 +14703,7 @@
       </c>
     </row>
     <row r="97" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="1">
         <v>45719</v>
       </c>
       <c r="B97">
@@ -14905,7 +14852,7 @@
       </c>
     </row>
     <row r="98" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="1">
         <v>45720</v>
       </c>
       <c r="B98">
@@ -15054,7 +15001,7 @@
       </c>
     </row>
     <row r="99" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="1">
         <v>45721</v>
       </c>
       <c r="B99">
@@ -15203,7 +15150,7 @@
       </c>
     </row>
     <row r="100" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="1">
         <v>45722</v>
       </c>
       <c r="B100">
@@ -15352,7 +15299,7 @@
       </c>
     </row>
     <row r="101" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="1">
         <v>45723</v>
       </c>
       <c r="B101">
@@ -15501,7 +15448,7 @@
       </c>
     </row>
     <row r="102" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="1">
         <v>45724</v>
       </c>
       <c r="B102">
@@ -15650,7 +15597,7 @@
       </c>
     </row>
     <row r="103" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="1">
         <v>45725</v>
       </c>
       <c r="B103">
@@ -15799,7 +15746,7 @@
       </c>
     </row>
     <row r="104" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="1">
         <v>45726</v>
       </c>
       <c r="B104">
@@ -15948,7 +15895,7 @@
       </c>
     </row>
     <row r="105" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="1">
         <v>45727</v>
       </c>
       <c r="B105">
@@ -16097,7 +16044,7 @@
       </c>
     </row>
     <row r="106" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="1">
         <v>45728</v>
       </c>
       <c r="B106">
@@ -16246,7 +16193,7 @@
       </c>
     </row>
     <row r="107" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="1">
         <v>45729</v>
       </c>
       <c r="B107">
@@ -16395,7 +16342,7 @@
       </c>
     </row>
     <row r="108" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="1">
         <v>45730</v>
       </c>
       <c r="B108">
@@ -16544,7 +16491,7 @@
       </c>
     </row>
     <row r="109" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="1">
         <v>45731</v>
       </c>
       <c r="B109">
@@ -16693,7 +16640,7 @@
       </c>
     </row>
     <row r="110" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="1">
         <v>45732</v>
       </c>
       <c r="B110">
@@ -16842,7 +16789,7 @@
       </c>
     </row>
     <row r="111" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="1">
         <v>45733</v>
       </c>
       <c r="B111">
@@ -16991,7 +16938,7 @@
       </c>
     </row>
     <row r="112" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="1">
         <v>45734</v>
       </c>
       <c r="B112">
@@ -17140,7 +17087,7 @@
       </c>
     </row>
     <row r="113" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="1">
         <v>45735</v>
       </c>
       <c r="B113">
@@ -17289,7 +17236,7 @@
       </c>
     </row>
     <row r="114" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="1">
         <v>45736</v>
       </c>
       <c r="B114">
@@ -17438,7 +17385,7 @@
       </c>
     </row>
     <row r="115" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="1">
         <v>45737</v>
       </c>
       <c r="B115">
@@ -17587,7 +17534,7 @@
       </c>
     </row>
     <row r="116" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="1">
         <v>45738</v>
       </c>
       <c r="B116">
@@ -17736,7 +17683,7 @@
       </c>
     </row>
     <row r="117" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="1">
         <v>45739</v>
       </c>
       <c r="B117">
@@ -17885,7 +17832,7 @@
       </c>
     </row>
     <row r="118" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="1">
         <v>45740</v>
       </c>
       <c r="B118">
@@ -18034,7 +17981,7 @@
       </c>
     </row>
     <row r="119" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="1">
         <v>45741</v>
       </c>
       <c r="B119">
@@ -18183,7 +18130,7 @@
       </c>
     </row>
     <row r="120" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="1">
         <v>45742</v>
       </c>
       <c r="B120">
@@ -18332,7 +18279,7 @@
       </c>
     </row>
     <row r="121" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="1">
         <v>45743</v>
       </c>
       <c r="B121">
@@ -18481,7 +18428,7 @@
       </c>
     </row>
     <row r="122" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="1">
         <v>45744</v>
       </c>
       <c r="B122">
@@ -18630,7 +18577,7 @@
       </c>
     </row>
     <row r="123" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="1">
         <v>45745</v>
       </c>
       <c r="B123">
@@ -18779,7 +18726,7 @@
       </c>
     </row>
     <row r="124" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="1">
         <v>45746</v>
       </c>
       <c r="B124">
@@ -18922,7 +18869,7 @@
       </c>
     </row>
     <row r="125" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="1">
         <v>45747</v>
       </c>
       <c r="B125">
@@ -19071,7 +19018,7 @@
       </c>
     </row>
     <row r="126" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="1">
         <v>45748</v>
       </c>
       <c r="B126">
@@ -19220,7 +19167,7 @@
       </c>
     </row>
     <row r="127" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="1">
         <v>45749</v>
       </c>
       <c r="B127">
@@ -19369,7 +19316,7 @@
       </c>
     </row>
     <row r="128" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="1">
         <v>45750</v>
       </c>
       <c r="B128">
@@ -19518,7 +19465,7 @@
       </c>
     </row>
     <row r="129" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+      <c r="A129" s="1">
         <v>45751</v>
       </c>
       <c r="B129">
@@ -19667,7 +19614,7 @@
       </c>
     </row>
     <row r="130" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+      <c r="A130" s="1">
         <v>45752</v>
       </c>
       <c r="B130">
@@ -19816,7 +19763,7 @@
       </c>
     </row>
     <row r="131" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+      <c r="A131" s="1">
         <v>45753</v>
       </c>
       <c r="B131">
@@ -19965,7 +19912,7 @@
       </c>
     </row>
     <row r="132" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+      <c r="A132" s="1">
         <v>45754</v>
       </c>
       <c r="B132">
@@ -20114,7 +20061,7 @@
       </c>
     </row>
     <row r="133" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+      <c r="A133" s="1">
         <v>45755</v>
       </c>
       <c r="B133">
@@ -20263,7 +20210,7 @@
       </c>
     </row>
     <row r="134" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+      <c r="A134" s="1">
         <v>45756</v>
       </c>
       <c r="B134">
@@ -20412,7 +20359,7 @@
       </c>
     </row>
     <row r="135" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+      <c r="A135" s="1">
         <v>45757</v>
       </c>
       <c r="B135">
@@ -20561,7 +20508,7 @@
       </c>
     </row>
     <row r="136" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+      <c r="A136" s="1">
         <v>45758</v>
       </c>
       <c r="B136">
@@ -20710,7 +20657,7 @@
       </c>
     </row>
     <row r="137" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+      <c r="A137" s="1">
         <v>45759</v>
       </c>
       <c r="B137">
@@ -20859,7 +20806,7 @@
       </c>
     </row>
     <row r="138" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+      <c r="A138" s="1">
         <v>45760</v>
       </c>
       <c r="B138">
@@ -21008,7 +20955,7 @@
       </c>
     </row>
     <row r="139" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+      <c r="A139" s="1">
         <v>45761</v>
       </c>
       <c r="B139">
@@ -21157,7 +21104,7 @@
       </c>
     </row>
     <row r="140" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+      <c r="A140" s="1">
         <v>45762</v>
       </c>
       <c r="B140">
@@ -21306,7 +21253,7 @@
       </c>
     </row>
     <row r="141" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+      <c r="A141" s="1">
         <v>45763</v>
       </c>
       <c r="B141">
@@ -21455,7 +21402,7 @@
       </c>
     </row>
     <row r="142" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+      <c r="A142" s="1">
         <v>45764</v>
       </c>
       <c r="B142">
@@ -21604,7 +21551,7 @@
       </c>
     </row>
     <row r="143" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+      <c r="A143" s="1">
         <v>45765</v>
       </c>
       <c r="B143">
@@ -21753,7 +21700,7 @@
       </c>
     </row>
     <row r="144" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+      <c r="A144" s="1">
         <v>45766</v>
       </c>
       <c r="B144">
@@ -21902,7 +21849,7 @@
       </c>
     </row>
     <row r="145" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+      <c r="A145" s="1">
         <v>45767</v>
       </c>
       <c r="B145">
@@ -22051,7 +21998,7 @@
       </c>
     </row>
     <row r="146" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+      <c r="A146" s="1">
         <v>45768</v>
       </c>
       <c r="B146">
@@ -22200,7 +22147,7 @@
       </c>
     </row>
     <row r="147" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+      <c r="A147" s="1">
         <v>45769</v>
       </c>
       <c r="B147">
@@ -22349,7 +22296,7 @@
       </c>
     </row>
     <row r="148" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+      <c r="A148" s="1">
         <v>45770</v>
       </c>
       <c r="B148">
@@ -22498,7 +22445,7 @@
       </c>
     </row>
     <row r="149" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+      <c r="A149" s="1">
         <v>45771</v>
       </c>
       <c r="B149">
@@ -22647,7 +22594,7 @@
       </c>
     </row>
     <row r="150" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+      <c r="A150" s="1">
         <v>45772</v>
       </c>
       <c r="B150">
@@ -22796,7 +22743,7 @@
       </c>
     </row>
     <row r="151" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+      <c r="A151" s="1">
         <v>45773</v>
       </c>
       <c r="B151">
@@ -22945,7 +22892,7 @@
       </c>
     </row>
     <row r="152" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+      <c r="A152" s="1">
         <v>45774</v>
       </c>
       <c r="B152">
@@ -23094,7 +23041,7 @@
       </c>
     </row>
     <row r="153" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+      <c r="A153" s="1">
         <v>45775</v>
       </c>
       <c r="B153">
@@ -23243,7 +23190,7 @@
       </c>
     </row>
     <row r="154" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+      <c r="A154" s="1">
         <v>45776</v>
       </c>
       <c r="B154">
@@ -23392,7 +23339,7 @@
       </c>
     </row>
     <row r="155" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+      <c r="A155" s="1">
         <v>45777</v>
       </c>
       <c r="B155">
@@ -23541,7 +23488,7 @@
       </c>
     </row>
     <row r="156" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+      <c r="A156" s="1">
         <v>45778</v>
       </c>
       <c r="B156">
@@ -23690,7 +23637,7 @@
       </c>
     </row>
     <row r="157" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+      <c r="A157" s="1">
         <v>45779</v>
       </c>
       <c r="B157">
@@ -23839,7 +23786,7 @@
       </c>
     </row>
     <row r="158" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+      <c r="A158" s="1">
         <v>45780</v>
       </c>
       <c r="B158">
@@ -23988,7 +23935,7 @@
       </c>
     </row>
     <row r="159" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+      <c r="A159" s="1">
         <v>45781</v>
       </c>
       <c r="B159">
@@ -24137,7 +24084,7 @@
       </c>
     </row>
     <row r="160" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+      <c r="A160" s="1">
         <v>45782</v>
       </c>
       <c r="B160">
@@ -24286,7 +24233,7 @@
       </c>
     </row>
     <row r="161" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+      <c r="A161" s="1">
         <v>45783</v>
       </c>
       <c r="B161">
@@ -24435,7 +24382,7 @@
       </c>
     </row>
     <row r="162" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+      <c r="A162" s="1">
         <v>45784</v>
       </c>
       <c r="B162">
@@ -24584,7 +24531,7 @@
       </c>
     </row>
     <row r="163" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+      <c r="A163" s="1">
         <v>45785</v>
       </c>
       <c r="B163">
@@ -24733,7 +24680,7 @@
       </c>
     </row>
     <row r="164" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+      <c r="A164" s="1">
         <v>45786</v>
       </c>
       <c r="B164">
@@ -24882,7 +24829,7 @@
       </c>
     </row>
     <row r="165" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+      <c r="A165" s="1">
         <v>45787</v>
       </c>
       <c r="B165">
@@ -25031,7 +24978,7 @@
       </c>
     </row>
     <row r="166" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+      <c r="A166" s="1">
         <v>45788</v>
       </c>
       <c r="B166">
@@ -25180,7 +25127,7 @@
       </c>
     </row>
     <row r="167" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+      <c r="A167" s="1">
         <v>45789</v>
       </c>
       <c r="B167">
@@ -25329,7 +25276,7 @@
       </c>
     </row>
     <row r="168" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+      <c r="A168" s="1">
         <v>45790</v>
       </c>
       <c r="B168">
@@ -25478,7 +25425,7 @@
       </c>
     </row>
     <row r="169" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+      <c r="A169" s="1">
         <v>45791</v>
       </c>
       <c r="B169">
@@ -25627,7 +25574,7 @@
       </c>
     </row>
     <row r="170" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+      <c r="A170" s="1">
         <v>45792</v>
       </c>
       <c r="B170">
@@ -25776,7 +25723,7 @@
       </c>
     </row>
     <row r="171" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+      <c r="A171" s="1">
         <v>45793</v>
       </c>
       <c r="B171">
@@ -25925,7 +25872,7 @@
       </c>
     </row>
     <row r="172" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+      <c r="A172" s="1">
         <v>45794</v>
       </c>
       <c r="B172">
@@ -26074,7 +26021,7 @@
       </c>
     </row>
     <row r="173" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+      <c r="A173" s="1">
         <v>45795</v>
       </c>
       <c r="B173">
@@ -26223,7 +26170,7 @@
       </c>
     </row>
     <row r="174" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+      <c r="A174" s="1">
         <v>45796</v>
       </c>
       <c r="B174">
@@ -26372,7 +26319,7 @@
       </c>
     </row>
     <row r="175" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+      <c r="A175" s="1">
         <v>45797</v>
       </c>
       <c r="B175">
@@ -26521,7 +26468,7 @@
       </c>
     </row>
     <row r="176" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+      <c r="A176" s="1">
         <v>45798</v>
       </c>
       <c r="B176">
@@ -26670,7 +26617,7 @@
       </c>
     </row>
     <row r="177" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+      <c r="A177" s="1">
         <v>45799</v>
       </c>
       <c r="B177">
@@ -26819,7 +26766,7 @@
       </c>
     </row>
     <row r="178" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+      <c r="A178" s="1">
         <v>45800</v>
       </c>
       <c r="B178">
@@ -26968,7 +26915,7 @@
       </c>
     </row>
     <row r="179" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+      <c r="A179" s="1">
         <v>45801</v>
       </c>
       <c r="B179">
@@ -27117,7 +27064,7 @@
       </c>
     </row>
     <row r="180" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A180" s="1">
         <v>45802</v>
       </c>
       <c r="B180">
@@ -27266,7 +27213,7 @@
       </c>
     </row>
     <row r="181" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+      <c r="A181" s="1">
         <v>45803</v>
       </c>
       <c r="B181">
@@ -27415,7 +27362,7 @@
       </c>
     </row>
     <row r="182" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+      <c r="A182" s="1">
         <v>45804</v>
       </c>
       <c r="B182">
@@ -27564,7 +27511,7 @@
       </c>
     </row>
     <row r="183" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+      <c r="A183" s="1">
         <v>45805</v>
       </c>
       <c r="B183">
@@ -27713,7 +27660,7 @@
       </c>
     </row>
     <row r="184" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+      <c r="A184" s="1">
         <v>45806</v>
       </c>
       <c r="B184">
@@ -27862,7 +27809,7 @@
       </c>
     </row>
     <row r="185" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+      <c r="A185" s="1">
         <v>45807</v>
       </c>
       <c r="B185">
@@ -28011,7 +27958,7 @@
       </c>
     </row>
     <row r="186" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+      <c r="A186" s="1">
         <v>45808</v>
       </c>
       <c r="B186">
@@ -28160,7 +28107,7 @@
       </c>
     </row>
     <row r="187" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+      <c r="A187" s="1">
         <v>45809</v>
       </c>
       <c r="B187">
@@ -28309,7 +28256,7 @@
       </c>
     </row>
     <row r="188" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+      <c r="A188" s="1">
         <v>45810</v>
       </c>
       <c r="B188">
@@ -28458,7 +28405,7 @@
       </c>
     </row>
     <row r="189" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+      <c r="A189" s="1">
         <v>45811</v>
       </c>
       <c r="B189">
@@ -28607,7 +28554,7 @@
       </c>
     </row>
     <row r="190" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+      <c r="A190" s="1">
         <v>45812</v>
       </c>
       <c r="B190">
@@ -28756,7 +28703,7 @@
       </c>
     </row>
     <row r="191" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+      <c r="A191" s="1">
         <v>45813</v>
       </c>
       <c r="B191">
@@ -28905,7 +28852,7 @@
       </c>
     </row>
     <row r="192" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+      <c r="A192" s="1">
         <v>45814</v>
       </c>
       <c r="B192">
@@ -29054,7 +29001,7 @@
       </c>
     </row>
     <row r="193" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+      <c r="A193" s="1">
         <v>45815</v>
       </c>
       <c r="B193">
@@ -29203,7 +29150,7 @@
       </c>
     </row>
     <row r="194" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+      <c r="A194" s="1">
         <v>45816</v>
       </c>
       <c r="B194">
@@ -29352,7 +29299,7 @@
       </c>
     </row>
     <row r="195" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+      <c r="A195" s="1">
         <v>45817</v>
       </c>
       <c r="B195">
@@ -29501,7 +29448,7 @@
       </c>
     </row>
     <row r="196" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+      <c r="A196" s="1">
         <v>45818</v>
       </c>
       <c r="B196">
@@ -29650,7 +29597,7 @@
       </c>
     </row>
     <row r="197" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+      <c r="A197" s="1">
         <v>45819</v>
       </c>
       <c r="B197">
@@ -29799,7 +29746,7 @@
       </c>
     </row>
     <row r="198" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+      <c r="A198" s="1">
         <v>45820</v>
       </c>
       <c r="B198">
@@ -29948,7 +29895,7 @@
       </c>
     </row>
     <row r="199" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+      <c r="A199" s="1">
         <v>45821</v>
       </c>
       <c r="B199">
@@ -30097,7 +30044,7 @@
       </c>
     </row>
     <row r="200" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+      <c r="A200" s="1">
         <v>45822</v>
       </c>
       <c r="B200">
@@ -30246,7 +30193,7 @@
       </c>
     </row>
     <row r="201" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+      <c r="A201" s="1">
         <v>45823</v>
       </c>
       <c r="B201">
@@ -30395,7 +30342,7 @@
       </c>
     </row>
     <row r="202" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="1">
         <v>45824</v>
       </c>
       <c r="B202">
@@ -30544,7 +30491,7 @@
       </c>
     </row>
     <row r="203" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+      <c r="A203" s="1">
         <v>45825</v>
       </c>
       <c r="B203">
@@ -30693,7 +30640,7 @@
       </c>
     </row>
     <row r="204" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+      <c r="A204" s="1">
         <v>45826</v>
       </c>
       <c r="B204">
@@ -30842,7 +30789,7 @@
       </c>
     </row>
     <row r="205" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+      <c r="A205" s="1">
         <v>45827</v>
       </c>
       <c r="B205">
@@ -30991,7 +30938,7 @@
       </c>
     </row>
     <row r="206" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+      <c r="A206" s="1">
         <v>45828</v>
       </c>
       <c r="B206">
@@ -31140,7 +31087,7 @@
       </c>
     </row>
     <row r="207" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+      <c r="A207" s="1">
         <v>45829</v>
       </c>
       <c r="B207">
@@ -31289,7 +31236,7 @@
       </c>
     </row>
     <row r="208" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+      <c r="A208" s="1">
         <v>45830</v>
       </c>
       <c r="B208">
@@ -31438,7 +31385,7 @@
       </c>
     </row>
     <row r="209" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+      <c r="A209" s="1">
         <v>45831</v>
       </c>
       <c r="B209">
@@ -31587,7 +31534,7 @@
       </c>
     </row>
     <row r="210" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A210" s="2">
+      <c r="A210" s="1">
         <v>45832</v>
       </c>
       <c r="B210">
@@ -31736,7 +31683,7 @@
       </c>
     </row>
     <row r="211" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A211" s="2">
+      <c r="A211" s="1">
         <v>45833</v>
       </c>
       <c r="B211">
@@ -31885,7 +31832,7 @@
       </c>
     </row>
     <row r="212" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A212" s="2">
+      <c r="A212" s="1">
         <v>45834</v>
       </c>
       <c r="B212">
@@ -32034,7 +31981,7 @@
       </c>
     </row>
     <row r="213" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+      <c r="A213" s="1">
         <v>45835</v>
       </c>
       <c r="B213">
@@ -32183,7 +32130,7 @@
       </c>
     </row>
     <row r="214" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A214" s="2">
+      <c r="A214" s="1">
         <v>45836</v>
       </c>
       <c r="B214">
@@ -32332,7 +32279,7 @@
       </c>
     </row>
     <row r="215" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A215" s="2">
+      <c r="A215" s="1">
         <v>45837</v>
       </c>
       <c r="B215">
@@ -32481,7 +32428,7 @@
       </c>
     </row>
     <row r="216" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A216" s="2">
+      <c r="A216" s="1">
         <v>45838</v>
       </c>
       <c r="B216">
@@ -32630,7 +32577,7 @@
       </c>
     </row>
     <row r="217" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A217" s="2">
+      <c r="A217" s="1">
         <v>45839</v>
       </c>
       <c r="B217">
@@ -32779,7 +32726,7 @@
       </c>
     </row>
     <row r="218" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A218" s="2">
+      <c r="A218" s="1">
         <v>45840</v>
       </c>
       <c r="B218">
@@ -32928,7 +32875,7 @@
       </c>
     </row>
     <row r="219" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A219" s="2">
+      <c r="A219" s="1">
         <v>45841</v>
       </c>
       <c r="B219">
@@ -33077,7 +33024,7 @@
       </c>
     </row>
     <row r="220" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A220" s="2">
+      <c r="A220" s="1">
         <v>45842</v>
       </c>
       <c r="B220">
@@ -33226,7 +33173,7 @@
       </c>
     </row>
     <row r="221" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A221" s="2">
+      <c r="A221" s="1">
         <v>45843</v>
       </c>
       <c r="B221">
@@ -33375,7 +33322,7 @@
       </c>
     </row>
     <row r="222" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A222" s="2">
+      <c r="A222" s="1">
         <v>45844</v>
       </c>
       <c r="B222">
@@ -33524,7 +33471,7 @@
       </c>
     </row>
     <row r="223" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A223" s="2">
+      <c r="A223" s="1">
         <v>45845</v>
       </c>
       <c r="B223">
@@ -33673,7 +33620,7 @@
       </c>
     </row>
     <row r="224" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A224" s="2">
+      <c r="A224" s="1">
         <v>45846</v>
       </c>
       <c r="B224">
@@ -33822,7 +33769,7 @@
       </c>
     </row>
     <row r="225" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A225" s="2">
+      <c r="A225" s="1">
         <v>45847</v>
       </c>
       <c r="B225">
@@ -33971,7 +33918,7 @@
       </c>
     </row>
     <row r="226" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A226" s="2">
+      <c r="A226" s="1">
         <v>45848</v>
       </c>
       <c r="B226">
@@ -34120,7 +34067,7 @@
       </c>
     </row>
     <row r="227" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A227" s="2">
+      <c r="A227" s="1">
         <v>45849</v>
       </c>
       <c r="B227">
@@ -34269,7 +34216,7 @@
       </c>
     </row>
     <row r="228" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A228" s="2">
+      <c r="A228" s="1">
         <v>45850</v>
       </c>
       <c r="B228">
@@ -34418,7 +34365,7 @@
       </c>
     </row>
     <row r="229" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A229" s="2">
+      <c r="A229" s="1">
         <v>45851</v>
       </c>
       <c r="B229">
@@ -34567,7 +34514,7 @@
       </c>
     </row>
     <row r="230" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A230" s="2">
+      <c r="A230" s="1">
         <v>45852</v>
       </c>
       <c r="B230">
@@ -34716,7 +34663,7 @@
       </c>
     </row>
     <row r="231" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A231" s="2">
+      <c r="A231" s="1">
         <v>45853</v>
       </c>
       <c r="B231">
@@ -34865,7 +34812,7 @@
       </c>
     </row>
     <row r="232" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A232" s="2">
+      <c r="A232" s="1">
         <v>45854</v>
       </c>
       <c r="B232">
@@ -35014,7 +34961,7 @@
       </c>
     </row>
     <row r="233" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A233" s="2">
+      <c r="A233" s="1">
         <v>45855</v>
       </c>
       <c r="B233">
@@ -35163,7 +35110,7 @@
       </c>
     </row>
     <row r="234" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A234" s="2">
+      <c r="A234" s="1">
         <v>45856</v>
       </c>
       <c r="B234">
@@ -35312,7 +35259,7 @@
       </c>
     </row>
     <row r="235" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A235" s="2">
+      <c r="A235" s="1">
         <v>45857</v>
       </c>
       <c r="B235">
@@ -35461,7 +35408,7 @@
       </c>
     </row>
     <row r="236" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A236" s="2">
+      <c r="A236" s="1">
         <v>45858</v>
       </c>
       <c r="B236">
@@ -35610,7 +35557,7 @@
       </c>
     </row>
     <row r="237" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A237" s="2">
+      <c r="A237" s="1">
         <v>45859</v>
       </c>
       <c r="B237">
@@ -35759,7 +35706,7 @@
       </c>
     </row>
     <row r="238" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A238" s="2">
+      <c r="A238" s="1">
         <v>45860</v>
       </c>
       <c r="B238">
@@ -35908,7 +35855,7 @@
       </c>
     </row>
     <row r="239" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A239" s="2">
+      <c r="A239" s="1">
         <v>45861</v>
       </c>
       <c r="B239">
@@ -36057,7 +36004,7 @@
       </c>
     </row>
     <row r="240" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A240" s="2">
+      <c r="A240" s="1">
         <v>45862</v>
       </c>
       <c r="B240">
@@ -36206,7 +36153,7 @@
       </c>
     </row>
     <row r="241" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A241" s="2">
+      <c r="A241" s="1">
         <v>45863</v>
       </c>
       <c r="B241">
@@ -36355,7 +36302,7 @@
       </c>
     </row>
     <row r="242" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A242" s="2">
+      <c r="A242" s="1">
         <v>45864</v>
       </c>
       <c r="B242">
@@ -36504,7 +36451,7 @@
       </c>
     </row>
     <row r="243" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A243" s="2">
+      <c r="A243" s="1">
         <v>45865</v>
       </c>
       <c r="B243">
@@ -36653,7 +36600,7 @@
       </c>
     </row>
     <row r="244" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A244" s="2">
+      <c r="A244" s="1">
         <v>45866</v>
       </c>
       <c r="B244">
@@ -36802,7 +36749,7 @@
       </c>
     </row>
     <row r="245" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A245" s="2">
+      <c r="A245" s="1">
         <v>45867</v>
       </c>
       <c r="B245">
@@ -36951,7 +36898,7 @@
       </c>
     </row>
     <row r="246" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A246" s="2">
+      <c r="A246" s="1">
         <v>45868</v>
       </c>
       <c r="B246">
@@ -37100,7 +37047,7 @@
       </c>
     </row>
     <row r="247" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A247" s="2">
+      <c r="A247" s="1">
         <v>45869</v>
       </c>
       <c r="B247">
@@ -37249,7 +37196,7 @@
       </c>
     </row>
     <row r="248" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A248" s="2">
+      <c r="A248" s="1">
         <v>45870</v>
       </c>
       <c r="B248">
@@ -37398,7 +37345,7 @@
       </c>
     </row>
     <row r="249" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A249" s="2">
+      <c r="A249" s="1">
         <v>45871</v>
       </c>
       <c r="B249">
@@ -37547,7 +37494,7 @@
       </c>
     </row>
     <row r="250" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A250" s="2">
+      <c r="A250" s="1">
         <v>45872</v>
       </c>
       <c r="B250">
@@ -37696,7 +37643,7 @@
       </c>
     </row>
     <row r="251" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A251" s="2">
+      <c r="A251" s="1">
         <v>45873</v>
       </c>
       <c r="B251">
@@ -37845,7 +37792,7 @@
       </c>
     </row>
     <row r="252" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A252" s="2">
+      <c r="A252" s="1">
         <v>45874</v>
       </c>
       <c r="B252">
@@ -37994,7 +37941,7 @@
       </c>
     </row>
     <row r="253" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A253" s="2">
+      <c r="A253" s="1">
         <v>45875</v>
       </c>
       <c r="B253">
@@ -38143,7 +38090,7 @@
       </c>
     </row>
     <row r="254" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A254" s="2">
+      <c r="A254" s="1">
         <v>45876</v>
       </c>
       <c r="B254">
@@ -38292,7 +38239,7 @@
       </c>
     </row>
     <row r="255" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A255" s="2">
+      <c r="A255" s="1">
         <v>45877</v>
       </c>
       <c r="B255">
@@ -38441,7 +38388,7 @@
       </c>
     </row>
     <row r="256" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A256" s="2">
+      <c r="A256" s="1">
         <v>45878</v>
       </c>
       <c r="B256">
@@ -38590,7 +38537,7 @@
       </c>
     </row>
     <row r="257" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A257" s="2">
+      <c r="A257" s="1">
         <v>45879</v>
       </c>
       <c r="B257">
@@ -38739,7 +38686,7 @@
       </c>
     </row>
     <row r="258" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A258" s="2">
+      <c r="A258" s="1">
         <v>45880</v>
       </c>
       <c r="B258">
@@ -38888,7 +38835,7 @@
       </c>
     </row>
     <row r="259" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A259" s="2">
+      <c r="A259" s="1">
         <v>45881</v>
       </c>
       <c r="B259">
@@ -39037,7 +38984,7 @@
       </c>
     </row>
     <row r="260" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A260" s="2">
+      <c r="A260" s="1">
         <v>45882</v>
       </c>
       <c r="B260">
@@ -39186,7 +39133,7 @@
       </c>
     </row>
     <row r="261" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A261" s="2">
+      <c r="A261" s="1">
         <v>45883</v>
       </c>
       <c r="B261">
@@ -39335,7 +39282,7 @@
       </c>
     </row>
     <row r="262" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A262" s="2">
+      <c r="A262" s="1">
         <v>45884</v>
       </c>
       <c r="B262">
@@ -39484,7 +39431,7 @@
       </c>
     </row>
     <row r="263" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
+      <c r="A263" s="1">
         <v>45885</v>
       </c>
       <c r="B263">
@@ -39633,7 +39580,7 @@
       </c>
     </row>
     <row r="264" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
+      <c r="A264" s="1">
         <v>45886</v>
       </c>
       <c r="B264">
@@ -39782,7 +39729,7 @@
       </c>
     </row>
     <row r="265" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
+      <c r="A265" s="1">
         <v>45887</v>
       </c>
       <c r="B265">
@@ -39931,7 +39878,7 @@
       </c>
     </row>
     <row r="266" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
+      <c r="A266" s="1">
         <v>45888</v>
       </c>
       <c r="B266">
@@ -40080,7 +40027,7 @@
       </c>
     </row>
     <row r="267" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
+      <c r="A267" s="1">
         <v>45889</v>
       </c>
       <c r="B267">
@@ -40229,7 +40176,7 @@
       </c>
     </row>
     <row r="268" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
+      <c r="A268" s="1">
         <v>45890</v>
       </c>
       <c r="B268">
@@ -40378,7 +40325,7 @@
       </c>
     </row>
     <row r="269" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
+      <c r="A269" s="1">
         <v>45891</v>
       </c>
       <c r="B269">
@@ -40527,7 +40474,7 @@
       </c>
     </row>
     <row r="270" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
+      <c r="A270" s="1">
         <v>45892</v>
       </c>
       <c r="B270">
@@ -40676,7 +40623,7 @@
       </c>
     </row>
     <row r="271" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
+      <c r="A271" s="1">
         <v>45893</v>
       </c>
       <c r="B271">
@@ -40825,7 +40772,7 @@
       </c>
     </row>
     <row r="272" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
+      <c r="A272" s="1">
         <v>45894</v>
       </c>
       <c r="B272">
@@ -40974,7 +40921,7 @@
       </c>
     </row>
     <row r="273" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
+      <c r="A273" s="1">
         <v>45895</v>
       </c>
       <c r="B273">
@@ -41123,7 +41070,7 @@
       </c>
     </row>
     <row r="274" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
+      <c r="A274" s="1">
         <v>45896</v>
       </c>
       <c r="B274">
@@ -41272,7 +41219,7 @@
       </c>
     </row>
     <row r="275" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
+      <c r="A275" s="1">
         <v>45897</v>
       </c>
       <c r="B275">
@@ -41421,7 +41368,7 @@
       </c>
     </row>
     <row r="276" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
+      <c r="A276" s="1">
         <v>45898</v>
       </c>
       <c r="B276">
@@ -41570,7 +41517,7 @@
       </c>
     </row>
     <row r="277" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
+      <c r="A277" s="1">
         <v>45899</v>
       </c>
       <c r="B277">
@@ -41719,7 +41666,7 @@
       </c>
     </row>
     <row r="278" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
+      <c r="A278" s="1">
         <v>45900</v>
       </c>
       <c r="B278">
@@ -41868,7 +41815,7 @@
       </c>
     </row>
     <row r="279" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
+      <c r="A279" s="1">
         <v>45901</v>
       </c>
       <c r="B279">
@@ -42017,7 +41964,7 @@
       </c>
     </row>
     <row r="280" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
+      <c r="A280" s="1">
         <v>45902</v>
       </c>
       <c r="B280">
@@ -42166,7 +42113,7 @@
       </c>
     </row>
     <row r="281" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
+      <c r="A281" s="1">
         <v>45903</v>
       </c>
       <c r="B281">
@@ -42315,7 +42262,7 @@
       </c>
     </row>
     <row r="282" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
+      <c r="A282" s="1">
         <v>45904</v>
       </c>
       <c r="B282">
@@ -42464,7 +42411,7 @@
       </c>
     </row>
     <row r="283" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
+      <c r="A283" s="1">
         <v>45905</v>
       </c>
       <c r="B283">
@@ -42613,7 +42560,7 @@
       </c>
     </row>
     <row r="284" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
+      <c r="A284" s="1">
         <v>45906</v>
       </c>
       <c r="B284">
@@ -42762,7 +42709,7 @@
       </c>
     </row>
     <row r="285" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
+      <c r="A285" s="1">
         <v>45907</v>
       </c>
       <c r="B285">
@@ -42911,7 +42858,7 @@
       </c>
     </row>
     <row r="286" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
+      <c r="A286" s="1">
         <v>45908</v>
       </c>
       <c r="B286">
@@ -43060,7 +43007,7 @@
       </c>
     </row>
     <row r="287" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
+      <c r="A287" s="1">
         <v>45909</v>
       </c>
       <c r="B287">
@@ -43209,7 +43156,7 @@
       </c>
     </row>
     <row r="288" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
+      <c r="A288" s="1">
         <v>45910</v>
       </c>
       <c r="B288">
@@ -43358,7 +43305,7 @@
       </c>
     </row>
     <row r="289" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
+      <c r="A289" s="1">
         <v>45911</v>
       </c>
       <c r="B289">
@@ -43507,7 +43454,7 @@
       </c>
     </row>
     <row r="290" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
+      <c r="A290" s="1">
         <v>45912</v>
       </c>
       <c r="B290">
@@ -43656,7 +43603,7 @@
       </c>
     </row>
     <row r="291" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
+      <c r="A291" s="1">
         <v>45913</v>
       </c>
       <c r="B291">
@@ -43805,7 +43752,7 @@
       </c>
     </row>
     <row r="292" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
+      <c r="A292" s="1">
         <v>45914</v>
       </c>
       <c r="B292">
@@ -43954,7 +43901,7 @@
       </c>
     </row>
     <row r="293" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
+      <c r="A293" s="1">
         <v>45915</v>
       </c>
       <c r="B293">
@@ -44103,7 +44050,7 @@
       </c>
     </row>
     <row r="294" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
+      <c r="A294" s="1">
         <v>45916</v>
       </c>
       <c r="B294">
@@ -44252,7 +44199,7 @@
       </c>
     </row>
     <row r="295" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
+      <c r="A295" s="1">
         <v>45917</v>
       </c>
       <c r="B295">
@@ -44401,7 +44348,7 @@
       </c>
     </row>
     <row r="296" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
+      <c r="A296" s="1">
         <v>45918</v>
       </c>
       <c r="B296">
@@ -44550,7 +44497,7 @@
       </c>
     </row>
     <row r="297" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
+      <c r="A297" s="1">
         <v>45919</v>
       </c>
       <c r="B297">
@@ -44699,7 +44646,7 @@
       </c>
     </row>
     <row r="298" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
+      <c r="A298" s="1">
         <v>45920</v>
       </c>
       <c r="B298">
@@ -44848,7 +44795,7 @@
       </c>
     </row>
     <row r="299" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
+      <c r="A299" s="1">
         <v>45921</v>
       </c>
       <c r="B299">
@@ -44997,7 +44944,7 @@
       </c>
     </row>
     <row r="300" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
+      <c r="A300" s="1">
         <v>45922</v>
       </c>
       <c r="B300">
@@ -45146,7 +45093,7 @@
       </c>
     </row>
     <row r="301" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
+      <c r="A301" s="1">
         <v>45923</v>
       </c>
       <c r="B301">
@@ -45295,7 +45242,7 @@
       </c>
     </row>
     <row r="302" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
+      <c r="A302" s="1">
         <v>45924</v>
       </c>
       <c r="B302">
@@ -45444,7 +45391,7 @@
       </c>
     </row>
     <row r="303" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
+      <c r="A303" s="1">
         <v>45925</v>
       </c>
       <c r="B303">
@@ -45593,7 +45540,7 @@
       </c>
     </row>
     <row r="304" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
+      <c r="A304" s="1">
         <v>45926</v>
       </c>
       <c r="B304">
@@ -45742,7 +45689,7 @@
       </c>
     </row>
     <row r="305" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A305" s="2">
+      <c r="A305" s="1">
         <v>45927</v>
       </c>
       <c r="B305">
@@ -45891,7 +45838,7 @@
       </c>
     </row>
     <row r="306" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A306" s="2">
+      <c r="A306" s="1">
         <v>45928</v>
       </c>
       <c r="B306">
@@ -46040,7 +45987,7 @@
       </c>
     </row>
     <row r="307" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A307" s="2">
+      <c r="A307" s="1">
         <v>45929</v>
       </c>
       <c r="B307">
@@ -46189,7 +46136,7 @@
       </c>
     </row>
     <row r="308" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A308" s="2">
+      <c r="A308" s="1">
         <v>45930</v>
       </c>
       <c r="B308">
@@ -46338,7 +46285,7 @@
       </c>
     </row>
     <row r="309" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A309" s="2">
+      <c r="A309" s="1">
         <v>45931</v>
       </c>
       <c r="B309">
@@ -46487,7 +46434,7 @@
       </c>
     </row>
     <row r="310" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A310" s="2">
+      <c r="A310" s="1">
         <v>45932</v>
       </c>
       <c r="B310">
@@ -46636,7 +46583,7 @@
       </c>
     </row>
     <row r="311" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A311" s="2">
+      <c r="A311" s="1">
         <v>45933</v>
       </c>
       <c r="B311">
@@ -46785,7 +46732,7 @@
       </c>
     </row>
     <row r="312" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
+      <c r="A312" s="1">
         <v>45934</v>
       </c>
       <c r="B312">
@@ -46934,7 +46881,7 @@
       </c>
     </row>
     <row r="313" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
+      <c r="A313" s="1">
         <v>45935</v>
       </c>
       <c r="B313">
@@ -47083,7 +47030,7 @@
       </c>
     </row>
     <row r="314" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A314" s="2">
+      <c r="A314" s="1">
         <v>45936</v>
       </c>
       <c r="B314">
@@ -47232,7 +47179,7 @@
       </c>
     </row>
     <row r="315" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A315" s="2">
+      <c r="A315" s="1">
         <v>45937</v>
       </c>
       <c r="B315">
@@ -47381,7 +47328,7 @@
       </c>
     </row>
     <row r="316" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A316" s="2">
+      <c r="A316" s="1">
         <v>45938</v>
       </c>
       <c r="B316">
@@ -47530,7 +47477,7 @@
       </c>
     </row>
     <row r="317" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A317" s="2">
+      <c r="A317" s="1">
         <v>45939</v>
       </c>
       <c r="B317">
@@ -47679,7 +47626,7 @@
       </c>
     </row>
     <row r="318" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A318" s="2">
+      <c r="A318" s="1">
         <v>45940</v>
       </c>
       <c r="B318">
@@ -47828,7 +47775,7 @@
       </c>
     </row>
     <row r="319" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A319" s="2">
+      <c r="A319" s="1">
         <v>45941</v>
       </c>
       <c r="B319">
@@ -47977,7 +47924,7 @@
       </c>
     </row>
     <row r="320" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A320" s="2">
+      <c r="A320" s="1">
         <v>45942</v>
       </c>
       <c r="B320">
@@ -48126,7 +48073,7 @@
       </c>
     </row>
     <row r="321" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A321" s="2">
+      <c r="A321" s="1">
         <v>45943</v>
       </c>
       <c r="B321">
@@ -48275,7 +48222,7 @@
       </c>
     </row>
     <row r="322" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A322" s="2">
+      <c r="A322" s="1">
         <v>45944</v>
       </c>
       <c r="B322">
@@ -48424,7 +48371,7 @@
       </c>
     </row>
     <row r="323" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A323" s="2">
+      <c r="A323" s="1">
         <v>45945</v>
       </c>
       <c r="B323">
@@ -48573,7 +48520,7 @@
       </c>
     </row>
     <row r="324" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A324" s="2">
+      <c r="A324" s="1">
         <v>45946</v>
       </c>
       <c r="B324">
@@ -48722,7 +48669,7 @@
       </c>
     </row>
     <row r="325" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A325" s="2">
+      <c r="A325" s="1">
         <v>45947</v>
       </c>
       <c r="B325">
@@ -48871,7 +48818,7 @@
       </c>
     </row>
     <row r="326" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
+      <c r="A326" s="1">
         <v>45948</v>
       </c>
       <c r="B326">
@@ -49020,7 +48967,7 @@
       </c>
     </row>
     <row r="327" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
+      <c r="A327" s="1">
         <v>45949</v>
       </c>
       <c r="B327">
@@ -49169,7 +49116,7 @@
       </c>
     </row>
     <row r="328" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
+      <c r="A328" s="1">
         <v>45950</v>
       </c>
       <c r="B328">
@@ -49318,7 +49265,7 @@
       </c>
     </row>
     <row r="329" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
+      <c r="A329" s="1">
         <v>45951</v>
       </c>
       <c r="B329">
@@ -49467,7 +49414,7 @@
       </c>
     </row>
     <row r="330" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A330" s="2">
+      <c r="A330" s="1">
         <v>45952</v>
       </c>
       <c r="B330">
@@ -49616,7 +49563,7 @@
       </c>
     </row>
     <row r="331" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A331" s="2">
+      <c r="A331" s="1">
         <v>45953</v>
       </c>
       <c r="B331">
@@ -49765,7 +49712,7 @@
       </c>
     </row>
     <row r="332" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A332" s="2">
+      <c r="A332" s="1">
         <v>45954</v>
       </c>
       <c r="B332">
@@ -49914,7 +49861,7 @@
       </c>
     </row>
     <row r="333" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A333" s="2">
+      <c r="A333" s="1">
         <v>45955</v>
       </c>
       <c r="B333">
@@ -50063,7 +50010,7 @@
       </c>
     </row>
     <row r="334" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A334" s="2">
+      <c r="A334" s="1">
         <v>45956</v>
       </c>
       <c r="B334">
@@ -50212,7 +50159,7 @@
       </c>
     </row>
     <row r="335" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A335" s="2">
+      <c r="A335" s="1">
         <v>45957</v>
       </c>
       <c r="B335">
@@ -50361,7 +50308,7 @@
       </c>
     </row>
     <row r="336" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A336" s="2">
+      <c r="A336" s="1">
         <v>45958</v>
       </c>
       <c r="B336">
@@ -50510,7 +50457,7 @@
       </c>
     </row>
     <row r="337" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A337" s="2">
+      <c r="A337" s="1">
         <v>45959</v>
       </c>
       <c r="B337">
@@ -50659,7 +50606,7 @@
       </c>
     </row>
     <row r="338" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A338" s="2">
+      <c r="A338" s="1">
         <v>45960</v>
       </c>
       <c r="B338">
@@ -50808,7 +50755,7 @@
       </c>
     </row>
     <row r="339" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
+      <c r="A339" s="1">
         <v>45961</v>
       </c>
       <c r="B339">
@@ -50957,7 +50904,7 @@
       </c>
     </row>
     <row r="340" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A340" s="2">
+      <c r="A340" s="1">
         <v>45962</v>
       </c>
       <c r="B340">
@@ -51106,7 +51053,7 @@
       </c>
     </row>
     <row r="341" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A341" s="2">
+      <c r="A341" s="1">
         <v>45963</v>
       </c>
       <c r="B341">
@@ -51255,7 +51202,7 @@
       </c>
     </row>
     <row r="342" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A342" s="2">
+      <c r="A342" s="1">
         <v>45964</v>
       </c>
       <c r="B342">
@@ -51404,7 +51351,7 @@
       </c>
     </row>
     <row r="343" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A343" s="2">
+      <c r="A343" s="1">
         <v>45965</v>
       </c>
       <c r="B343">
@@ -51553,7 +51500,7 @@
       </c>
     </row>
     <row r="344" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A344" s="2">
+      <c r="A344" s="1">
         <v>45966</v>
       </c>
       <c r="B344">
@@ -51702,7 +51649,7 @@
       </c>
     </row>
     <row r="345" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A345" s="2">
+      <c r="A345" s="1">
         <v>45967</v>
       </c>
       <c r="B345">
@@ -51851,7 +51798,7 @@
       </c>
     </row>
     <row r="346" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A346" s="2">
+      <c r="A346" s="1">
         <v>45968</v>
       </c>
       <c r="B346">
@@ -52000,7 +51947,7 @@
       </c>
     </row>
     <row r="347" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A347" s="2">
+      <c r="A347" s="1">
         <v>45969</v>
       </c>
       <c r="B347">
@@ -52149,7 +52096,7 @@
       </c>
     </row>
     <row r="348" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A348" s="2">
+      <c r="A348" s="1">
         <v>45970</v>
       </c>
       <c r="B348">
@@ -52298,7 +52245,7 @@
       </c>
     </row>
     <row r="349" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A349" s="2">
+      <c r="A349" s="1">
         <v>45971</v>
       </c>
       <c r="B349">
@@ -52447,7 +52394,7 @@
       </c>
     </row>
     <row r="350" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A350" s="2">
+      <c r="A350" s="1">
         <v>45972</v>
       </c>
       <c r="B350">
@@ -52596,7 +52543,7 @@
       </c>
     </row>
     <row r="351" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A351" s="2">
+      <c r="A351" s="1">
         <v>45973</v>
       </c>
       <c r="B351">
@@ -52745,7 +52692,7 @@
       </c>
     </row>
     <row r="352" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A352" s="2">
+      <c r="A352" s="1">
         <v>45974</v>
       </c>
       <c r="B352">
@@ -52894,7 +52841,7 @@
       </c>
     </row>
     <row r="353" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A353" s="2">
+      <c r="A353" s="1">
         <v>45975</v>
       </c>
       <c r="B353">
@@ -53043,7 +52990,7 @@
       </c>
     </row>
     <row r="354" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A354" s="2">
+      <c r="A354" s="1">
         <v>45976</v>
       </c>
       <c r="B354">
@@ -53192,7 +53139,7 @@
       </c>
     </row>
     <row r="355" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A355" s="2">
+      <c r="A355" s="1">
         <v>45977</v>
       </c>
       <c r="B355">
@@ -53341,7 +53288,7 @@
       </c>
     </row>
     <row r="356" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A356" s="2">
+      <c r="A356" s="1">
         <v>45978</v>
       </c>
       <c r="B356">
@@ -53490,7 +53437,7 @@
       </c>
     </row>
     <row r="357" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A357" s="2">
+      <c r="A357" s="1">
         <v>45979</v>
       </c>
       <c r="B357">
@@ -53639,7 +53586,7 @@
       </c>
     </row>
     <row r="358" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A358" s="2">
+      <c r="A358" s="1">
         <v>45980</v>
       </c>
       <c r="B358">
@@ -53788,7 +53735,7 @@
       </c>
     </row>
     <row r="359" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A359" s="2">
+      <c r="A359" s="1">
         <v>45981</v>
       </c>
       <c r="B359">
@@ -53937,7 +53884,7 @@
       </c>
     </row>
     <row r="360" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A360" s="2">
+      <c r="A360" s="1">
         <v>45982</v>
       </c>
       <c r="B360">
@@ -54086,7 +54033,7 @@
       </c>
     </row>
     <row r="361" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A361" s="2">
+      <c r="A361" s="1">
         <v>45983</v>
       </c>
       <c r="B361">
@@ -54235,7 +54182,7 @@
       </c>
     </row>
     <row r="362" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A362" s="2">
+      <c r="A362" s="1">
         <v>45984</v>
       </c>
       <c r="B362">
@@ -54384,7 +54331,7 @@
       </c>
     </row>
     <row r="363" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A363" s="2">
+      <c r="A363" s="1">
         <v>45985</v>
       </c>
       <c r="B363">
@@ -54533,7 +54480,7 @@
       </c>
     </row>
     <row r="364" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A364" s="2">
+      <c r="A364" s="1">
         <v>45986</v>
       </c>
       <c r="B364">
@@ -54682,7 +54629,7 @@
       </c>
     </row>
     <row r="365" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A365" s="2">
+      <c r="A365" s="1">
         <v>45987</v>
       </c>
       <c r="B365">
@@ -54830,370 +54777,8 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="366" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A366" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B366" s="3">
-        <f>SUM(B2:B365)</f>
-        <v>223.85700000000011</v>
-      </c>
-      <c r="C366" s="3">
-        <f>SUM(C2:C365)</f>
-        <v>216.27999999999997</v>
-      </c>
-      <c r="D366" s="3">
-        <f>SUM(D2:D365)</f>
-        <v>202.00900000000004</v>
-      </c>
-      <c r="E366" s="3">
-        <f t="shared" ref="E366:AW366" si="0">SUM(E2:E365)</f>
-        <v>197.95599999999988</v>
-      </c>
-      <c r="F366" s="3">
-        <f t="shared" si="0"/>
-        <v>198.02500000000001</v>
-      </c>
-      <c r="G366" s="3">
-        <f t="shared" si="0"/>
-        <v>194.36000000000004</v>
-      </c>
-      <c r="H366" s="3">
-        <f t="shared" si="0"/>
-        <v>191.33900000000008</v>
-      </c>
-      <c r="I366" s="3">
-        <f t="shared" si="0"/>
-        <v>189.80599999999995</v>
-      </c>
-      <c r="J366" s="3">
-        <f t="shared" si="0"/>
-        <v>185.6810000000001</v>
-      </c>
-      <c r="K366" s="3">
-        <f t="shared" si="0"/>
-        <v>182.16300000000007</v>
-      </c>
-      <c r="L366" s="3">
-        <f t="shared" si="0"/>
-        <v>218.57999999999996</v>
-      </c>
-      <c r="M366" s="3">
-        <f t="shared" si="0"/>
-        <v>268.25200000000018</v>
-      </c>
-      <c r="N366" s="3">
-        <f t="shared" si="0"/>
-        <v>282.36800000000011</v>
-      </c>
-      <c r="O366" s="3">
-        <f t="shared" si="0"/>
-        <v>301.48500000000018</v>
-      </c>
-      <c r="P366" s="3">
-        <f t="shared" si="0"/>
-        <v>311.47599999999989</v>
-      </c>
-      <c r="Q366" s="3">
-        <f t="shared" si="0"/>
-        <v>299.48699999999997</v>
-      </c>
-      <c r="R366" s="3">
-        <f t="shared" si="0"/>
-        <v>299.45399999999989</v>
-      </c>
-      <c r="S366" s="3">
-        <f t="shared" si="0"/>
-        <v>273.14699999999976</v>
-      </c>
-      <c r="T366" s="3">
-        <f t="shared" si="0"/>
-        <v>230.29899999999995</v>
-      </c>
-      <c r="U366" s="3">
-        <f t="shared" si="0"/>
-        <v>169.07500000000005</v>
-      </c>
-      <c r="V366" s="3">
-        <f t="shared" si="0"/>
-        <v>138.71899999999994</v>
-      </c>
-      <c r="W366" s="3">
-        <f t="shared" si="0"/>
-        <v>102.45500000000003</v>
-      </c>
-      <c r="X366" s="3">
-        <f t="shared" si="0"/>
-        <v>89.493000000000009</v>
-      </c>
-      <c r="Y366" s="3">
-        <f t="shared" si="0"/>
-        <v>93.96899999999998</v>
-      </c>
-      <c r="Z366" s="3">
-        <f t="shared" si="0"/>
-        <v>101.27000000000012</v>
-      </c>
-      <c r="AA366" s="3">
-        <f t="shared" si="0"/>
-        <v>94.011999999999944</v>
-      </c>
-      <c r="AB366" s="3">
-        <f t="shared" si="0"/>
-        <v>85.591000000000037</v>
-      </c>
-      <c r="AC366" s="3">
-        <f t="shared" si="0"/>
-        <v>95.646000000000086</v>
-      </c>
-      <c r="AD366" s="3">
-        <f t="shared" si="0"/>
-        <v>100.30399999999999</v>
-      </c>
-      <c r="AE366" s="3">
-        <f t="shared" si="0"/>
-        <v>105.16900000000004</v>
-      </c>
-      <c r="AF366" s="3">
-        <f t="shared" si="0"/>
-        <v>123.04000000000002</v>
-      </c>
-      <c r="AG366" s="3">
-        <f t="shared" si="0"/>
-        <v>163.22700000000012</v>
-      </c>
-      <c r="AH366" s="3">
-        <f t="shared" si="0"/>
-        <v>221.37599999999998</v>
-      </c>
-      <c r="AI366" s="3">
-        <f t="shared" si="0"/>
-        <v>228.45700000000011</v>
-      </c>
-      <c r="AJ366" s="3">
-        <f t="shared" si="0"/>
-        <v>218.88899999999984</v>
-      </c>
-      <c r="AK366" s="3">
-        <f t="shared" si="0"/>
-        <v>245.69900000000007</v>
-      </c>
-      <c r="AL366" s="3">
-        <f t="shared" si="0"/>
-        <v>243.37499999999974</v>
-      </c>
-      <c r="AM366" s="3">
-        <f t="shared" si="0"/>
-        <v>247.50999999999976</v>
-      </c>
-      <c r="AN366" s="3">
-        <f t="shared" si="0"/>
-        <v>253.97300000000004</v>
-      </c>
-      <c r="AO366" s="3">
-        <f t="shared" si="0"/>
-        <v>265.12100000000015</v>
-      </c>
-      <c r="AP366" s="3">
-        <f t="shared" si="0"/>
-        <v>276.17200000000003</v>
-      </c>
-      <c r="AQ366" s="3">
-        <f t="shared" si="0"/>
-        <v>302.61799999999999</v>
-      </c>
-      <c r="AR366" s="3">
-        <f t="shared" si="0"/>
-        <v>396.61499999999995</v>
-      </c>
-      <c r="AS366" s="3">
-        <f t="shared" si="0"/>
-        <v>418.11400000000026</v>
-      </c>
-      <c r="AT366" s="3">
-        <f t="shared" si="0"/>
-        <v>407.41899999999987</v>
-      </c>
-      <c r="AU366" s="3">
-        <f t="shared" si="0"/>
-        <v>340.81800000000038</v>
-      </c>
-      <c r="AV366" s="3">
-        <f t="shared" si="0"/>
-        <v>280.60300000000001</v>
-      </c>
-      <c r="AW366" s="3">
-        <f t="shared" si="0"/>
-        <v>243.43199999999993</v>
-      </c>
-    </row>
-    <row r="367" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A367" s="7"/>
-      <c r="B367" s="8">
-        <v>0</v>
-      </c>
-      <c r="C367" s="8">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D367" s="8">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E367" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F367" s="8">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G367" s="8">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="H367" s="8">
-        <v>0.125</v>
-      </c>
-      <c r="I367" s="8">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="J367" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K367" s="8">
-        <v>0.1875</v>
-      </c>
-      <c r="L367" s="8">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="M367" s="8">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="N367" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="O367" s="8">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="P367" s="8">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="Q367" s="8">
-        <v>0.3125</v>
-      </c>
-      <c r="R367" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="S367" s="8">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="T367" s="8">
-        <v>0.375</v>
-      </c>
-      <c r="U367" s="8">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="V367" s="8">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="W367" s="8">
-        <v>0.4375</v>
-      </c>
-      <c r="X367" s="8">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="Y367" s="8">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="Z367" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="AA367" s="8">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="AB367" s="8">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="AC367" s="8">
-        <v>0.5625</v>
-      </c>
-      <c r="AD367" s="8">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="AE367" s="8">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="AF367" s="8">
-        <v>0.625</v>
-      </c>
-      <c r="AG367" s="8">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="AH367" s="8">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="AI367" s="8">
-        <v>0.6875</v>
-      </c>
-      <c r="AJ367" s="8">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="AK367" s="8">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="AL367" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="AM367" s="8">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="AN367" s="8">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="AO367" s="8">
-        <v>0.8125</v>
-      </c>
-      <c r="AP367" s="8">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="AQ367" s="8">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="AR367" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="AS367" s="8">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="AT367" s="8">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="AU367" s="8">
-        <v>0.9375</v>
-      </c>
-      <c r="AV367" s="8">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="AW367" s="8">
-        <v>0.97916666666666663</v>
-      </c>
-    </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A369" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B369" s="10"/>
-      <c r="C369" s="11">
-        <f>SUM(B366:AW366)</f>
-        <v>10518.185000000001</v>
-      </c>
-      <c r="D369" s="11"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A369:B369"/>
-    <mergeCell ref="C369:D369"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B366 C366:AW366" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>